<commit_message>
Modified schema, added changes for modularity and scalabilty
</commit_message>
<xml_diff>
--- a/project/app/data/biology.xlsx
+++ b/project/app/data/biology.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lambe\OneDrive\Documents\Courses\2023-2024\Semester 2\COMP3901\FST-Degree-Planner\project\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945B877A-4ED8-464F-B035-0ADD8DF6B3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BBC673-E5B9-4888-AD93-520E4549484F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="105">
   <si>
     <r>
       <rPr>
@@ -1202,6 +1202,9 @@
   </si>
   <si>
     <t>BIOC3014</t>
+  </si>
+  <si>
+    <t>ANTI-REQUISITE</t>
   </si>
 </sst>
 </file>
@@ -1735,10 +1738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1750,14 +1753,14 @@
     <col min="5" max="5" width="10.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" style="1" customWidth="1"/>
     <col min="7" max="7" width="48.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.44140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.77734375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="9" width="20.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.77734375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>68</v>
       </c>
@@ -1779,20 +1782,23 @@
       <c r="G1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>49</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1818,16 +1824,19 @@
         <v>59</v>
       </c>
       <c r="I2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="L2" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
@@ -1853,16 +1862,19 @@
         <v>59</v>
       </c>
       <c r="I3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="L3" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
@@ -1888,16 +1900,19 @@
         <v>53</v>
       </c>
       <c r="I4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="K4" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="L4" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
@@ -1923,16 +1938,19 @@
         <v>59</v>
       </c>
       <c r="I5" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="K5" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="L5" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -1958,16 +1976,19 @@
         <v>54</v>
       </c>
       <c r="I6" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="K6" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="L6" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
@@ -1991,16 +2012,19 @@
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="L7" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
@@ -2026,16 +2050,19 @@
         <v>56</v>
       </c>
       <c r="I8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="L8" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
@@ -2061,16 +2088,19 @@
         <v>56</v>
       </c>
       <c r="I9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="K9" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="L9" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>18</v>
       </c>
@@ -2096,16 +2126,19 @@
         <v>59</v>
       </c>
       <c r="I10" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="K10" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="L10" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
@@ -2131,16 +2164,19 @@
         <v>59</v>
       </c>
       <c r="I11" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="K11" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="L11" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>103</v>
       </c>
@@ -2166,16 +2202,19 @@
         <v>59</v>
       </c>
       <c r="I12" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="K12" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="L12" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>26</v>
       </c>
@@ -2201,16 +2240,19 @@
         <v>59</v>
       </c>
       <c r="I13" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="K13" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="L13" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>28</v>
       </c>
@@ -2236,16 +2278,19 @@
         <v>59</v>
       </c>
       <c r="I14" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="K14" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="L14" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>30</v>
       </c>
@@ -2271,16 +2316,19 @@
         <v>59</v>
       </c>
       <c r="I15" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="K15" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="14" t="s">
+      <c r="L15" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>32</v>
       </c>
@@ -2306,16 +2354,19 @@
         <v>59</v>
       </c>
       <c r="I16" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J16" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="K16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K16" s="14" t="s">
+      <c r="L16" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>34</v>
       </c>
@@ -2341,16 +2392,19 @@
         <v>60</v>
       </c>
       <c r="I17" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J17" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="K17" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="L17" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>36</v>
       </c>
@@ -2376,16 +2430,19 @@
         <v>59</v>
       </c>
       <c r="I18" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J18" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="K18" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K18" s="14" t="s">
+      <c r="L18" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>38</v>
       </c>
@@ -2411,16 +2468,19 @@
         <v>59</v>
       </c>
       <c r="I19" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J19" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="K19" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K19" s="14" t="s">
+      <c r="L19" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>40</v>
       </c>
@@ -2446,16 +2506,19 @@
         <v>59</v>
       </c>
       <c r="I20" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="K20" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="L20" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>43</v>
       </c>
@@ -2481,16 +2544,19 @@
         <v>59</v>
       </c>
       <c r="I21" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J21" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="K21" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K21" s="14" t="s">
+      <c r="L21" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>46</v>
       </c>
@@ -2516,25 +2582,28 @@
         <v>59</v>
       </c>
       <c r="I22" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J22" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="K22" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K22" s="14" t="s">
+      <c r="L22" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:12" ht="28.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:12" ht="29.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:12" ht="31.8" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="29.4" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="30.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="29.4" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>